<commit_message>
Re-defined default model '2_sut_multi_year_rcot', deleted id from sets.
</commit_message>
<xml_diff>
--- a/default/2_sut_multi_year_rcot/sets.xlsx
+++ b/default/2_sut_multi_year_rcot/sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_sut_multi_year_rcot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E340E2-039D-462F-82C7-C9386200829A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84DBC8B-AB30-4659-9342-8C169AF95195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34980" yWindow="3420" windowWidth="28800" windowHeight="15430" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10250" yWindow="1340" windowWidth="21200" windowHeight="15370" tabRatio="902" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_SCENARIOS" sheetId="1" r:id="rId1"/>
@@ -25,41 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
-  <si>
-    <t>s_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>s_Name</t>
   </si>
   <si>
-    <t>y_ID</t>
-  </si>
-  <si>
     <t>y_Name</t>
   </si>
   <si>
-    <t>t_ID</t>
-  </si>
-  <si>
     <t>t_Name</t>
   </si>
   <si>
     <t>t_Category</t>
   </si>
   <si>
-    <t>f_ID</t>
-  </si>
-  <si>
     <t>f_Name</t>
   </si>
   <si>
     <t>f_Name_agg_1</t>
   </si>
   <si>
-    <t>c_ID</t>
-  </si>
-  <si>
     <t>c_Name</t>
   </si>
   <si>
@@ -109,9 +94,6 @@
   </si>
   <si>
     <t>operational cost</t>
-  </si>
-  <si>
-    <t>f_agg_ID</t>
   </si>
   <si>
     <t>f_agg_Name</t>
@@ -483,36 +465,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -520,125 +628,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -646,109 +653,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>